<commit_message>
Updated the Screener feature
</commit_message>
<xml_diff>
--- a/financial_models/Opportunities/6601.HK_Stock_Valuation.xlsx
+++ b/financial_models/Opportunities/6601.HK_Stock_Valuation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\Invest_Proc\financial_models\Opportunities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D924C7B-6941-4B38-8059-1A3D69A4190D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1D64E0-B453-40FD-B500-ADDB988CDC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -3940,179 +3940,6 @@
     <xf numFmtId="4" fontId="5" fillId="13" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="16" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="16" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="8" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="8" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="8" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="8" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="8" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="4" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="4" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4135,9 +3962,182 @@
     <xf numFmtId="8" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="4" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="4" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="8" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="8" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="16" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="16" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="8" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="8" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="8" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4562,8 +4562,8 @@
   </sheetPr>
   <dimension ref="A1:L966"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4607,27 +4607,27 @@
       <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="401" t="s">
+      <c r="C3" s="396" t="s">
         <v>334</v>
       </c>
-      <c r="D3" s="402"/>
+      <c r="D3" s="397"/>
       <c r="E3" s="15"/>
       <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="411" t="s">
+      <c r="I3" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="412"/>
+      <c r="J3" s="409"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="403" t="s">
+      <c r="C4" s="398" t="s">
         <v>335</v>
       </c>
-      <c r="D4" s="404"/>
+      <c r="D4" s="399"/>
       <c r="E4" s="6"/>
       <c r="G4" s="5" t="s">
         <v>5</v>
@@ -4644,10 +4644,10 @@
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="405">
+      <c r="C5" s="400">
         <v>44931</v>
       </c>
-      <c r="D5" s="404"/>
+      <c r="D5" s="399"/>
       <c r="E5" s="122" t="str">
         <f ca="1">IF(C5+30&gt;=TODAY(),"Patience Premium","")</f>
         <v/>
@@ -4655,10 +4655,10 @@
       <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="413">
+      <c r="I5" s="392">
         <v>1333330500</v>
       </c>
-      <c r="J5" s="414"/>
+      <c r="J5" s="393"/>
       <c r="K5" s="151"/>
       <c r="L5" s="85"/>
     </row>
@@ -4681,11 +4681,11 @@
         <v>9</v>
       </c>
       <c r="H6" s="133"/>
-      <c r="I6" s="415">
+      <c r="I6" s="410">
         <f>I4*I5/1000000</f>
         <v>2359.9949849999998</v>
       </c>
-      <c r="J6" s="416"/>
+      <c r="J6" s="411"/>
       <c r="K6" s="151"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
@@ -4759,30 +4759,30 @@
       <c r="B11" s="312" t="s">
         <v>267</v>
       </c>
-      <c r="C11" s="425">
+      <c r="C11" s="422">
         <f ca="1">C12-D10</f>
         <v>5.1000000000000004E-2</v>
       </c>
-      <c r="D11" s="426"/>
+      <c r="D11" s="423"/>
       <c r="E11" s="13"/>
       <c r="G11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="423" t="s">
+      <c r="I11" s="420" t="s">
         <v>336</v>
       </c>
-      <c r="J11" s="424"/>
+      <c r="J11" s="421"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" thickTop="1">
       <c r="B12" s="313" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="379">
+      <c r="C12" s="424">
         <f ca="1">IF(C10="CN",8%,6%)*IF($C$5+30&gt;=TODAY(),1.2,1)</f>
         <v>0.08</v>
       </c>
-      <c r="D12" s="380"/>
+      <c r="D12" s="425"/>
       <c r="G12" s="134" t="s">
         <v>16</v>
       </c>
@@ -4856,14 +4856,14 @@
         <f>I4</f>
         <v>1.77</v>
       </c>
-      <c r="C16" s="389">
+      <c r="C16" s="431">
         <v>0.1</v>
       </c>
       <c r="D16" s="159">
         <f>IF(B17='FCFF Model'!G29,"Net Asset", H14/B16-1-C16)</f>
         <v>-1.9833198710867889E-2</v>
       </c>
-      <c r="E16" s="384">
+      <c r="E16" s="428">
         <f>'FCFF Model'!D11*Exchange_Rate</f>
         <v>0.25194656451543168</v>
       </c>
@@ -4871,14 +4871,14 @@
         <f>E16/B16</f>
         <v>0.14234269181662806</v>
       </c>
-      <c r="G16" s="392" t="s">
+      <c r="G16" s="415" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="417">
+      <c r="H16" s="412">
         <f>('FCFF Model'!G19)*Exchange_Rate</f>
         <v>2.0424389077766301</v>
       </c>
-      <c r="I16" s="392" t="s">
+      <c r="I16" s="415" t="s">
         <v>26</v>
       </c>
       <c r="J16" s="206">
@@ -4891,19 +4891,19 @@
         <f>MAX(H14/(1+C16),'FCFF Model'!G29)</f>
         <v>1.7380865802561487</v>
       </c>
-      <c r="C17" s="390"/>
+      <c r="C17" s="432"/>
       <c r="D17" s="288">
         <f>IF(B17='FCFF Model'!G29,"Net Asset",H14/B17-1-C16)</f>
         <v>8.3266726846886741E-17</v>
       </c>
-      <c r="E17" s="385"/>
+      <c r="E17" s="429"/>
       <c r="F17" s="162">
         <f>E16/B17</f>
         <v>0.14495627972589337</v>
       </c>
-      <c r="G17" s="393"/>
-      <c r="H17" s="418"/>
-      <c r="I17" s="393"/>
+      <c r="G17" s="416"/>
+      <c r="H17" s="413"/>
+      <c r="I17" s="416"/>
       <c r="J17" s="205">
         <f>B17-$H$16</f>
         <v>-0.30435232752048136</v>
@@ -4914,19 +4914,19 @@
         <f>C35</f>
         <v>1.62</v>
       </c>
-      <c r="C18" s="391"/>
+      <c r="C18" s="433"/>
       <c r="D18" s="160">
         <f>IF(B17='FCFF Model'!G29,"NA: "&amp;ROUND('FCFF Model'!G29/B18-1,2)*100&amp;"%", H14/B18-1-C16)</f>
         <v>8.0182245852940509E-2</v>
       </c>
-      <c r="E18" s="386"/>
+      <c r="E18" s="430"/>
       <c r="F18" s="163">
         <f>E16/B18</f>
         <v>0.15552257068853806</v>
       </c>
-      <c r="G18" s="394"/>
-      <c r="H18" s="419"/>
-      <c r="I18" s="394"/>
+      <c r="G18" s="417"/>
+      <c r="H18" s="414"/>
+      <c r="I18" s="417"/>
       <c r="J18" s="207">
         <f>B18-$H$16</f>
         <v>-0.42243890777662996</v>
@@ -4959,52 +4959,52 @@
       <c r="B21" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="408" t="s">
+      <c r="C21" s="403" t="s">
         <v>337</v>
       </c>
-      <c r="D21" s="409"/>
-      <c r="E21" s="409"/>
-      <c r="F21" s="409"/>
-      <c r="G21" s="409"/>
-      <c r="H21" s="409"/>
-      <c r="I21" s="409"/>
-      <c r="J21" s="410"/>
+      <c r="D21" s="404"/>
+      <c r="E21" s="404"/>
+      <c r="F21" s="404"/>
+      <c r="G21" s="404"/>
+      <c r="H21" s="404"/>
+      <c r="I21" s="404"/>
+      <c r="J21" s="405"/>
     </row>
     <row r="22" spans="1:10" ht="52.5" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="421" t="s">
+      <c r="C22" s="419" t="s">
         <v>339</v>
       </c>
-      <c r="D22" s="422"/>
-      <c r="E22" s="422"/>
-      <c r="F22" s="422"/>
-      <c r="G22" s="421" t="s">
+      <c r="D22" s="384"/>
+      <c r="E22" s="384"/>
+      <c r="F22" s="384"/>
+      <c r="G22" s="419" t="s">
         <v>340</v>
       </c>
-      <c r="H22" s="421"/>
-      <c r="I22" s="422"/>
-      <c r="J22" s="422"/>
+      <c r="H22" s="419"/>
+      <c r="I22" s="384"/>
+      <c r="J22" s="384"/>
     </row>
     <row r="23" spans="1:10" ht="52.5" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="387" t="s">
+      <c r="C23" s="406" t="s">
         <v>341</v>
       </c>
-      <c r="D23" s="388"/>
-      <c r="E23" s="388"/>
-      <c r="F23" s="388"/>
-      <c r="G23" s="387" t="s">
+      <c r="D23" s="407"/>
+      <c r="E23" s="407"/>
+      <c r="F23" s="407"/>
+      <c r="G23" s="406" t="s">
         <v>342</v>
       </c>
-      <c r="H23" s="387"/>
-      <c r="I23" s="388"/>
-      <c r="J23" s="388"/>
+      <c r="H23" s="406"/>
+      <c r="I23" s="407"/>
+      <c r="J23" s="407"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="B24" s="6"/>
@@ -5048,207 +5048,207 @@
       <c r="B26" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="406">
+      <c r="C26" s="401">
         <v>44932</v>
       </c>
-      <c r="D26" s="407"/>
-      <c r="E26" s="398" t="str">
+      <c r="D26" s="402"/>
+      <c r="E26" s="437" t="str">
         <f>IF(C26="","","Action_Planning")</f>
         <v>Action_Planning</v>
       </c>
-      <c r="F26" s="399"/>
-      <c r="G26" s="399"/>
-      <c r="H26" s="400"/>
-      <c r="I26" s="420" t="s">
+      <c r="F26" s="438"/>
+      <c r="G26" s="438"/>
+      <c r="H26" s="439"/>
+      <c r="I26" s="418" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="420"/>
+      <c r="J26" s="418"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="B27" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="383">
+      <c r="C27" s="427">
         <f>C31/D25</f>
         <v>0.11666666666666667</v>
       </c>
       <c r="D27" s="382"/>
-      <c r="E27" s="381">
+      <c r="E27" s="426">
         <f>E31/D25</f>
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="F27" s="382"/>
-      <c r="G27" s="396">
+      <c r="G27" s="435">
         <f>G31/D25</f>
         <v>0</v>
       </c>
-      <c r="H27" s="397"/>
-      <c r="I27" s="395">
+      <c r="H27" s="436"/>
+      <c r="I27" s="434">
         <f>C27+E27+G27</f>
         <v>0.19766666666666666</v>
       </c>
-      <c r="J27" s="395"/>
+      <c r="J27" s="434"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
       <c r="B28" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="372">
+      <c r="C28" s="383">
         <v>40000</v>
       </c>
-      <c r="D28" s="422"/>
-      <c r="E28" s="372">
+      <c r="D28" s="384"/>
+      <c r="E28" s="383">
         <v>30000</v>
       </c>
-      <c r="F28" s="422"/>
-      <c r="G28" s="413"/>
-      <c r="H28" s="414"/>
-      <c r="I28" s="437">
+      <c r="F28" s="384"/>
+      <c r="G28" s="392"/>
+      <c r="H28" s="393"/>
+      <c r="I28" s="372">
         <f>C28+E28+G28</f>
         <v>70000</v>
       </c>
-      <c r="J28" s="437"/>
+      <c r="J28" s="372"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
       <c r="B29" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="447">
+      <c r="C29" s="385">
         <v>1.75</v>
       </c>
-      <c r="D29" s="422"/>
-      <c r="E29" s="447">
+      <c r="D29" s="384"/>
+      <c r="E29" s="385">
         <v>1.62</v>
       </c>
-      <c r="F29" s="422"/>
-      <c r="G29" s="427"/>
-      <c r="H29" s="428"/>
-      <c r="I29" s="433"/>
-      <c r="J29" s="433"/>
+      <c r="F29" s="384"/>
+      <c r="G29" s="386"/>
+      <c r="H29" s="387"/>
+      <c r="I29" s="394"/>
+      <c r="J29" s="394"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
       <c r="B30" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="435">
+      <c r="C30" s="370">
         <f>C29*$I$5/1000000</f>
         <v>2333.3283750000001</v>
       </c>
-      <c r="D30" s="442"/>
-      <c r="E30" s="435">
+      <c r="D30" s="377"/>
+      <c r="E30" s="370">
         <f>E29*$I$5/1000000</f>
         <v>2159.99541</v>
       </c>
-      <c r="F30" s="442"/>
-      <c r="G30" s="429">
+      <c r="F30" s="377"/>
+      <c r="G30" s="388">
         <f>G29*$I$5/1000000</f>
         <v>0</v>
       </c>
-      <c r="H30" s="430"/>
-      <c r="I30" s="434"/>
-      <c r="J30" s="434"/>
+      <c r="H30" s="389"/>
+      <c r="I30" s="395"/>
+      <c r="J30" s="395"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="443">
+      <c r="C31" s="378">
         <f>C28*C29</f>
         <v>70000</v>
       </c>
-      <c r="D31" s="444"/>
-      <c r="E31" s="436">
+      <c r="D31" s="379"/>
+      <c r="E31" s="371">
         <f>E28*E29</f>
         <v>48600</v>
       </c>
-      <c r="F31" s="445"/>
-      <c r="G31" s="431">
+      <c r="F31" s="380"/>
+      <c r="G31" s="390">
         <f>G28*G29</f>
         <v>0</v>
       </c>
-      <c r="H31" s="432"/>
-      <c r="I31" s="436">
+      <c r="H31" s="391"/>
+      <c r="I31" s="371">
         <f>C31+E31+G31</f>
         <v>118600</v>
       </c>
-      <c r="J31" s="436"/>
+      <c r="J31" s="371"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="438"/>
-      <c r="D32" s="439"/>
-      <c r="E32" s="446">
+      <c r="C32" s="373"/>
+      <c r="D32" s="374"/>
+      <c r="E32" s="381">
         <f>IF(C31=0,"-",(C31+E31)/(C28+E28))</f>
         <v>1.6942857142857144</v>
       </c>
       <c r="F32" s="382"/>
       <c r="G32" s="117"/>
       <c r="H32" s="117"/>
-      <c r="I32" s="446">
+      <c r="I32" s="381">
         <f>IF(I31=0,"",I31/I28)</f>
         <v>1.6942857142857144</v>
       </c>
-      <c r="J32" s="446"/>
+      <c r="J32" s="381"/>
     </row>
     <row r="33" spans="2:11" ht="15.75" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="440"/>
-      <c r="D33" s="441"/>
-      <c r="E33" s="435">
+      <c r="C33" s="375"/>
+      <c r="D33" s="376"/>
+      <c r="E33" s="370">
         <f>IF(E32="-","-",E32*$I$5/1000000)</f>
         <v>2259.0428185714286</v>
       </c>
-      <c r="F33" s="442"/>
+      <c r="F33" s="377"/>
       <c r="G33" s="118"/>
       <c r="H33" s="118"/>
-      <c r="I33" s="435">
+      <c r="I33" s="370">
         <f>IF(I32="","",I32*$I$5/1000000)</f>
         <v>2259.0428185714286</v>
       </c>
-      <c r="J33" s="435"/>
+      <c r="J33" s="370"/>
     </row>
     <row r="34" spans="2:11" ht="15.75" customHeight="1"/>
     <row r="35" spans="2:11" ht="15.75" customHeight="1">
       <c r="B35" s="146" t="s">
         <v>309</v>
       </c>
-      <c r="C35" s="370">
+      <c r="C35" s="440">
         <f>E29</f>
         <v>1.62</v>
       </c>
-      <c r="D35" s="371"/>
-      <c r="G35" s="374" t="s">
+      <c r="D35" s="441"/>
+      <c r="G35" s="443" t="s">
         <v>311</v>
       </c>
-      <c r="H35" s="375"/>
-      <c r="I35" s="370">
+      <c r="H35" s="444"/>
+      <c r="I35" s="440">
         <f>F14</f>
         <v>2.0424389077766301</v>
       </c>
-      <c r="J35" s="371"/>
+      <c r="J35" s="441"/>
     </row>
     <row r="36" spans="2:11" ht="15.75" customHeight="1">
       <c r="B36" s="146" t="s">
         <v>310</v>
       </c>
-      <c r="C36" s="372">
+      <c r="C36" s="383">
         <f>E28</f>
         <v>30000</v>
       </c>
-      <c r="D36" s="373"/>
-      <c r="G36" s="376" t="s">
+      <c r="D36" s="442"/>
+      <c r="G36" s="445" t="s">
         <v>321</v>
       </c>
-      <c r="H36" s="376"/>
-      <c r="I36" s="377">
+      <c r="H36" s="445"/>
+      <c r="I36" s="446">
         <f>IF(C26="",0,I35/C29-1)</f>
         <v>0.16710794730093137</v>
       </c>
-      <c r="J36" s="378"/>
+      <c r="J36" s="447"/>
     </row>
     <row r="37" spans="2:11" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:11" ht="15.75" customHeight="1">
@@ -6327,6 +6327,44 @@
     <row r="966" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I28:J28"/>
@@ -6343,44 +6381,6 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="B16">
@@ -10640,7 +10640,7 @@
         <f>SUM(I11:I13)+SUM(I28:I30)</f>
         <v>16614</v>
       </c>
-      <c r="E53" s="444"/>
+      <c r="E53" s="379"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="3" t="s">
@@ -10659,7 +10659,7 @@
       <c r="D54" s="456">
         <v>0</v>
       </c>
-      <c r="E54" s="422"/>
+      <c r="E54" s="384"/>
       <c r="F54" s="6" t="s">
         <v>132</v>
       </c>
@@ -10673,7 +10673,7 @@
       <c r="D55" s="456">
         <v>0</v>
       </c>
-      <c r="E55" s="422"/>
+      <c r="E55" s="384"/>
       <c r="F55" s="5" t="s">
         <v>133</v>
       </c>
@@ -10756,11 +10756,11 @@
       <c r="B63" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D63" s="377">
+      <c r="D63" s="446">
         <f>((C26-C11-C12-C14-C15-C16*G16-C19*G19-C20*G20)-I26)/Data!C7</f>
         <v>-0.16776182102549406</v>
       </c>
-      <c r="E63" s="378"/>
+      <c r="E63" s="447"/>
     </row>
     <row r="64" spans="2:9" ht="15" customHeight="1">
       <c r="B64" s="3" t="s">

</xml_diff>